<commit_message>
adding more test data and excel for manual project
</commit_message>
<xml_diff>
--- a/Database-test-case-(Sales-Customer).xlsx
+++ b/Database-test-case-(Sales-Customer).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IslamHassan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEPI_GP\open-cart-demo-online-shopping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB28F030-A195-49FF-829A-37490755A503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA599A1E-153B-4D61-98D3-1E3C23CF52A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F506F1E7-1669-43D9-8551-1234B563D8BA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F506F1E7-1669-43D9-8551-1234B563D8BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="91">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1443,13 +1443,161 @@
   </si>
   <si>
     <t>Updated Customer Email</t>
+  </si>
+  <si>
+    <t>DB-016</t>
+  </si>
+  <si>
+    <t>DB-017</t>
+  </si>
+  <si>
+    <t>DB-018</t>
+  </si>
+  <si>
+    <t>DB-019</t>
+  </si>
+  <si>
+    <t>SELECT * FROM oc_order_history WHERE order_id = 1 ORDER BY date_added DESC;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Verify Order History Log (Read)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Ensure order status updates are correctly saved.</t>
+    </r>
+  </si>
+  <si>
+    <t>Admin Order History should show the same latest status and comment.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Returned rows should match frontend: correct </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>order_status_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and comment text.</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify product stock reduces after purchase.</t>
+  </si>
+  <si>
+    <t>SELECT quantity FROM oc_product WHERE product_id = 40;</t>
+  </si>
+  <si>
+    <t>Product page should show reduced stock.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Quantity should be decreased by the exact ordered amount from </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>oc_order_product</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify shipping charge is correctly stored under order totals.</t>
+  </si>
+  <si>
+    <t>SELECT title, value FROM oc_order_total WHERE order_id = 1 AND code = 'shipping';</t>
+  </si>
+  <si>
+    <t>On order details page, shipping cost (e.g., “Flat Shipping Rate: $5.00”) is shown.</t>
+  </si>
+  <si>
+    <t>Query should return exactly one row:title = shipping method name (e.g., “Flat Shipping Rate”),value = shipping price (e.g., 5.00).</t>
+  </si>
+  <si>
+    <t>UPDATE oc_address SET city='NewCity' WHERE address_id = 1;  SELECT city FROM oc_address WHERE address_id = 1;</t>
+  </si>
+  <si>
+    <t>Update customer address and verify database update.</t>
+  </si>
+  <si>
+    <t>Customer Address Book displays the updated city.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The city field updates to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>NewCity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>oc_address</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1488,6 +1636,19 @@
       <color rgb="FF444746"/>
       <name val="Google Sans Text"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1537,41 +1698,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1906,349 +2047,442 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{017A6380-4848-4E03-8230-3A6010DCC5C1}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" customWidth="1"/>
-    <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.69921875" customWidth="1"/>
+    <col min="2" max="2" width="45.09765625" customWidth="1"/>
+    <col min="3" max="3" width="94.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.09765625" customWidth="1"/>
+    <col min="5" max="5" width="65" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" thickBot="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="93" customHeight="1" thickBot="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="57" customHeight="1" thickBot="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60" thickBot="1">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:6" ht="42" thickBot="1">
+      <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="58.5" thickBot="1">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:6" ht="28.2" thickBot="1">
+      <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="72.75" thickBot="1">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:6" ht="42" thickBot="1">
+      <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="72.75" thickBot="1">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:6" ht="42" thickBot="1">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="60" thickBot="1">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:6" ht="42" thickBot="1">
+      <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="72" thickBot="1">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:6" ht="55.8" thickBot="1">
+      <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="100.5" thickBot="1">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:6" ht="55.8" thickBot="1">
+      <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="89.25" thickBot="1">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:6" ht="55.8" thickBot="1">
+      <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="73.5" thickBot="1">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:6" ht="55.8" thickBot="1">
+      <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="115.5" thickBot="1">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:6" ht="55.8" thickBot="1">
+      <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="44.25" thickBot="1">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:6" ht="28.2" thickBot="1">
+      <c r="A15" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="59.25" thickBot="1">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:6" ht="42" thickBot="1">
+      <c r="A16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="4" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.2" thickBot="1">
+      <c r="A17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.2" thickBot="1">
+      <c r="A18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="42" thickBot="1">
+      <c r="A19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="28.2" thickBot="1">
+      <c r="A20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="C21" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A95317433F16A84E86C5BD170513CF32" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="465f8a72315053741d0bb1390d63bf9d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a1285e94-d8c3-4e5c-9ac5-21d2b8f33cfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="69b64cf170e112620a4780630ba75930" ns3:_="">
     <xsd:import namespace="a1285e94-d8c3-4e5c-9ac5-21d2b8f33cfd"/>
@@ -2398,15 +2632,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2414,6 +2639,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B30151-59CC-41DF-A395-CB998ACFB3C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0719CEB4-C716-46CF-BE0B-B05697814749}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2427,14 +2660,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B30151-59CC-41DF-A395-CB998ACFB3C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>